<commit_message>
Small changes to sprint 3 execution chart
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint3/execution.xlsx
+++ b/sprint_backlog/sprint3/execution.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2A2A95-0A4F-4EAC-BEFD-1A87615989B9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCB0542-F672-4961-B99B-5284361330B2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -170,9 +170,6 @@
     <t xml:space="preserve">Changes from Planning to Execution: </t>
   </si>
   <si>
-    <t>Saad was able to complete T13 instead of Won as well as his own assigned task (T14)</t>
-  </si>
-  <si>
     <t>Due to a misunderstanding Mo was not able to complete T9 completely and feels that he needs the next sprint to fully implement it</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>Alex was able to partially able complete T10 due to a limited time amount of time available because he had three midterms during the sprint duration. He will finish the remainder of the task during next sprint.</t>
+  </si>
+  <si>
+    <t>Saad is able to complete T13 instead of Won as well as his own assigned task (T14). He also thinks that it will only take 2 story points. He also believes that T15 will only take 3 story points as well.</t>
   </si>
 </sst>
 </file>
@@ -312,18 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -338,6 +326,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A23" sqref="A23:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,33 +739,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -824,7 +824,7 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -848,7 +848,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -898,7 +898,7 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -974,7 +974,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -992,135 +992,160 @@
       <c r="J11" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A23:J24"/>
+    <mergeCell ref="A17:J18"/>
+    <mergeCell ref="A19:J20"/>
+    <mergeCell ref="A21:J22"/>
+    <mergeCell ref="A15:J16"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A17:J18"/>
-    <mergeCell ref="A19:J20"/>
-    <mergeCell ref="A21:J22"/>
-    <mergeCell ref="A15:J16"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>